<commit_message>
updated chi2 and column list
</commit_message>
<xml_diff>
--- a/data_files/data_dictionary.xlsx
+++ b/data_files/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevineliasen/GoogleDrive/CodingStuff/Codeup/Capstone/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD35FD90-E762-1F4C-94F8-077101EA3152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E2223B-0A93-1147-9947-FA50C8B4E481}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{31CA8657-46A0-9D49-84BF-6461B50EDC7B}"/>
   </bookViews>
@@ -1246,8 +1246,8 @@
   <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1948,13 +1948,13 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G19" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="H19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J19" t="s">
         <v>6</v>
@@ -1983,13 +1983,13 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G20" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="H20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J20" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
updates to wrangle (added special encoding fields) AND explore (divide-by-zero error)
</commit_message>
<xml_diff>
--- a/data_files/data_dictionary.xlsx
+++ b/data_files/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevineliasen/GoogleDrive/CodingStuff/Codeup/Capstone/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B053066-D95B-1A42-B352-069525BC5324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C16C2D-6B72-0B42-9807-25229656C0CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{31CA8657-46A0-9D49-84BF-6461B50EDC7B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="315">
   <si>
     <t>survey_section</t>
   </si>
@@ -893,9 +893,6 @@
     <t>category</t>
   </si>
   <si>
-    <t>bool</t>
-  </si>
-  <si>
     <t>company_small</t>
   </si>
   <si>
@@ -950,15 +947,9 @@
     <t>Company has 51 or more researchers</t>
   </si>
   <si>
-    <t>q17tws</t>
-  </si>
-  <si>
     <t>q17cs1</t>
   </si>
   <si>
-    <t>q17cs0</t>
-  </si>
-  <si>
     <t>q17cs4</t>
   </si>
   <si>
@@ -984,6 +975,12 @@
   </si>
   <si>
     <t>Ideal conference has more than 500 attendees</t>
+  </si>
+  <si>
+    <t>q17cs2</t>
+  </si>
+  <si>
+    <t>q17cs3</t>
   </si>
 </sst>
 </file>
@@ -1336,8 +1333,8 @@
   <dimension ref="A1:L90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4127,7 +4124,7 @@
         <v>234</v>
       </c>
       <c r="H75" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I75" t="s">
         <v>275</v>
@@ -4241,7 +4238,7 @@
         <v>234</v>
       </c>
       <c r="H78" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I78" t="s">
         <v>278</v>
@@ -4279,7 +4276,7 @@
         <v>234</v>
       </c>
       <c r="H79" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I79" t="s">
         <v>278</v>
@@ -4317,7 +4314,7 @@
         <v>234</v>
       </c>
       <c r="H80" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I80" t="s">
         <v>278</v>
@@ -4334,10 +4331,10 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B81" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C81" t="b">
         <v>0</v>
@@ -4346,7 +4343,7 @@
         <v>0</v>
       </c>
       <c r="E81" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F81" t="s">
         <v>235</v>
@@ -4355,7 +4352,7 @@
         <v>234</v>
       </c>
       <c r="H81" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I81" t="s">
         <v>278</v>
@@ -4367,15 +4364,15 @@
         <v>6</v>
       </c>
       <c r="L81" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B82" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C82" t="b">
         <v>0</v>
@@ -4384,7 +4381,7 @@
         <v>0</v>
       </c>
       <c r="E82" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F82" t="s">
         <v>235</v>
@@ -4393,7 +4390,7 @@
         <v>234</v>
       </c>
       <c r="H82" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I82" t="s">
         <v>278</v>
@@ -4405,15 +4402,15 @@
         <v>6</v>
       </c>
       <c r="L82" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B83" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C83" t="b">
         <v>0</v>
@@ -4422,7 +4419,7 @@
         <v>0</v>
       </c>
       <c r="E83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83" t="s">
         <v>235</v>
@@ -4431,7 +4428,7 @@
         <v>234</v>
       </c>
       <c r="H83" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I83" t="s">
         <v>278</v>
@@ -4443,15 +4440,15 @@
         <v>6</v>
       </c>
       <c r="L83" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B84" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C84" t="b">
         <v>0</v>
@@ -4460,7 +4457,7 @@
         <v>0</v>
       </c>
       <c r="E84" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F84" t="s">
         <v>235</v>
@@ -4469,7 +4466,7 @@
         <v>234</v>
       </c>
       <c r="H84" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I84" t="s">
         <v>278</v>
@@ -4481,15 +4478,15 @@
         <v>6</v>
       </c>
       <c r="L84" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B85" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C85" t="b">
         <v>0</v>
@@ -4498,7 +4495,7 @@
         <v>0</v>
       </c>
       <c r="E85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F85" t="s">
         <v>235</v>
@@ -4507,7 +4504,7 @@
         <v>234</v>
       </c>
       <c r="H85" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I85" t="s">
         <v>278</v>
@@ -4519,15 +4516,15 @@
         <v>6</v>
       </c>
       <c r="L85" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B86" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C86" t="b">
         <v>0</v>
@@ -4536,7 +4533,7 @@
         <v>0</v>
       </c>
       <c r="E86" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" t="s">
         <v>235</v>
@@ -4545,7 +4542,7 @@
         <v>234</v>
       </c>
       <c r="H86" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I86" t="s">
         <v>278</v>
@@ -4557,15 +4554,15 @@
         <v>6</v>
       </c>
       <c r="L86" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B87" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C87" t="b">
         <v>0</v>
@@ -4574,7 +4571,7 @@
         <v>0</v>
       </c>
       <c r="E87" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" t="s">
         <v>235</v>
@@ -4583,7 +4580,7 @@
         <v>234</v>
       </c>
       <c r="H87" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I87" t="s">
         <v>278</v>
@@ -4595,15 +4592,15 @@
         <v>78</v>
       </c>
       <c r="L87" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
+        <v>313</v>
+      </c>
+      <c r="B88" t="s">
         <v>306</v>
-      </c>
-      <c r="B88" t="s">
-        <v>309</v>
       </c>
       <c r="C88" t="b">
         <v>0</v>
@@ -4612,7 +4609,7 @@
         <v>0</v>
       </c>
       <c r="E88" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F88" t="s">
         <v>235</v>
@@ -4621,7 +4618,7 @@
         <v>234</v>
       </c>
       <c r="H88" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I88" t="s">
         <v>278</v>
@@ -4633,15 +4630,15 @@
         <v>78</v>
       </c>
       <c r="L88" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="B89" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C89" t="b">
         <v>0</v>
@@ -4650,7 +4647,7 @@
         <v>0</v>
       </c>
       <c r="E89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F89" t="s">
         <v>235</v>
@@ -4659,7 +4656,7 @@
         <v>234</v>
       </c>
       <c r="H89" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I89" t="s">
         <v>278</v>
@@ -4671,15 +4668,15 @@
         <v>78</v>
       </c>
       <c r="L89" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B90" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C90" t="b">
         <v>0</v>
@@ -4688,7 +4685,7 @@
         <v>0</v>
       </c>
       <c r="E90" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F90" t="s">
         <v>235</v>
@@ -4697,7 +4694,7 @@
         <v>234</v>
       </c>
       <c r="H90" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I90" t="s">
         <v>278</v>
@@ -4709,7 +4706,7 @@
         <v>78</v>
       </c>
       <c r="L90" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed typo in wrangle
</commit_message>
<xml_diff>
--- a/data_files/data_dictionary.xlsx
+++ b/data_files/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevineliasen/GoogleDrive/CodingStuff/Codeup/Capstone/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C16C2D-6B72-0B42-9807-25229656C0CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F1B5CB-FC34-3940-B48C-86E3CF207426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{31CA8657-46A0-9D49-84BF-6461B50EDC7B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="319">
   <si>
     <t>survey_section</t>
   </si>
@@ -981,6 +981,18 @@
   </si>
   <si>
     <t>q17cs3</t>
+  </si>
+  <si>
+    <t>x02</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>float64</t>
+  </si>
+  <si>
+    <t>User has history of conferences and/or favors attending conferences to learn</t>
   </si>
 </sst>
 </file>
@@ -1330,11 +1342,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53992D9E-FAE0-004A-B683-F804D396F232}">
-  <dimension ref="A1:L90"/>
+  <dimension ref="A1:L91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A90" sqref="A90"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4709,6 +4721,41 @@
         <v>312</v>
       </c>
     </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A91" t="s">
+        <v>315</v>
+      </c>
+      <c r="B91" t="s">
+        <v>316</v>
+      </c>
+      <c r="C91" t="b">
+        <v>0</v>
+      </c>
+      <c r="D91" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" t="b">
+        <v>0</v>
+      </c>
+      <c r="F91" t="s">
+        <v>235</v>
+      </c>
+      <c r="G91" t="s">
+        <v>234</v>
+      </c>
+      <c r="H91" t="s">
+        <v>317</v>
+      </c>
+      <c r="J91" t="s">
+        <v>252</v>
+      </c>
+      <c r="K91" t="s">
+        <v>252</v>
+      </c>
+      <c r="L91" t="s">
+        <v>318</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L80" xr:uid="{914F26F1-26D3-3745-8C3E-01075C6E7E48}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated error in import data (questions 13e and 13f reversed)
</commit_message>
<xml_diff>
--- a/data_files/data_dictionary.xlsx
+++ b/data_files/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevineliasen/GoogleDrive/CodingStuff/Codeup/Capstone/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F0B1C8-3808-354A-A045-6131756E3CB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA95C49-9ECE-9C4E-8FBD-7A910278B629}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{31CA8657-46A0-9D49-84BF-6461B50EDC7B}"/>
   </bookViews>
@@ -1346,7 +1346,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>